<commit_message>
changed stock to holding
</commit_message>
<xml_diff>
--- a/test/buy_history.xlsx
+++ b/test/buy_history.xlsx
@@ -25,7 +25,7 @@
     <t>Cost</t>
   </si>
   <si>
-    <t>Stock</t>
+    <t>Holding</t>
   </si>
   <si>
     <t>Total</t>
@@ -174,16 +174,16 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -355,9 +355,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -437,7 +437,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -465,10 +465,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -724,9 +724,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1014,7 +1014,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1042,10 +1042,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>